<commit_message>
Add address of combo
</commit_message>
<xml_diff>
--- a/financialControl.xlsx
+++ b/financialControl.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>Day</t>
   </si>
@@ -52,15 +52,15 @@
   </si>
   <si>
     <t>Index rotary</t>
+  </si>
+  <si>
+    <t>https://vi.aliexpress.com/item/T-l-20-1-Worm-Loai-Reducer-NEMA23-Worm-Gear-ng-C-B-c-2-8Nm/32841463277.html?spm=2114.10010108.1000014.1.4b115c02F4k4fb&amp;pvid=08888958-1276-48d9-a3ec-0a2ff57c7cdb&amp;gps-id=pcDetailBottomMoreOtherSeller&amp;scm=1007.13338.120274.000000000000000&amp;scm-url=1007.13338.120274.000000000000000&amp;scm_id=1007.13338.120274.000000000000000&amp;fbclid=IwAR2NFrEzP0PjPCEgglo3cGtLrq7Lk6hBt9w-g9eAX3J8KnxGtHRJZ2_m_Kg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="dd/mm/yyyy"/>
-  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -93,7 +93,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -377,7 +377,7 @@
   <dimension ref="B2:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -434,6 +434,9 @@
       <c r="G3" t="s">
         <v>7</v>
       </c>
+      <c r="H3" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" s="1">

</xml_diff>

<commit_message>
add address of rotary
</commit_message>
<xml_diff>
--- a/financialControl.xlsx
+++ b/financialControl.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>Day</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>https://vi.aliexpress.com/item/T-l-20-1-Worm-Loai-Reducer-NEMA23-Worm-Gear-ng-C-B-c-2-8Nm/32841463277.html?spm=2114.10010108.1000014.1.4b115c02F4k4fb&amp;pvid=08888958-1276-48d9-a3ec-0a2ff57c7cdb&amp;gps-id=pcDetailBottomMoreOtherSeller&amp;scm=1007.13338.120274.000000000000000&amp;scm-url=1007.13338.120274.000000000000000&amp;scm_id=1007.13338.120274.000000000000000&amp;fbclid=IwAR2NFrEzP0PjPCEgglo3cGtLrq7Lk6hBt9w-g9eAX3J8KnxGtHRJZ2_m_Kg</t>
+  </si>
+  <si>
+    <t>Duong Ba Trac</t>
   </si>
 </sst>
 </file>
@@ -377,7 +380,7 @@
   <dimension ref="B2:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -458,6 +461,9 @@
       <c r="G4" t="s">
         <v>7</v>
       </c>
+      <c r="H4" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="I10" t="s">

</xml_diff>